<commit_message>
Added more lines to DCRS data
</commit_message>
<xml_diff>
--- a/Extract from DCRS.xlsx
+++ b/Extract from DCRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\HDS-Week-2---GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDD0135-834A-4811-9294-24CE8F69BF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9143F184-2D6D-4267-BFDB-8B93C2493666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>Client ID</t>
   </si>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,7 +397,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>12345</v>
+        <v>12346</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>12345</v>
+        <v>12347</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -419,7 +419,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>12345</v>
+        <v>12348</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>12345</v>
+        <v>12349</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -441,7 +441,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>12345</v>
+        <v>12350</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>12345</v>
+        <v>12351</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>12345</v>
+        <v>12352</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -474,13 +474,101 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>12345</v>
+        <v>12353</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>45901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>12354</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12355</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45962</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12356</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12357</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>12358</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>12359</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>46082</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>12360</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>46113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>12361</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>46143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>